<commit_message>
chore(data): fix Excel header ' brand' -> 'brand' in public/stock/stock_20_0.xlsx
</commit_message>
<xml_diff>
--- a/public/stock/stock_20_0.xlsx
+++ b/public/stock/stock_20_0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\IMG汽配\imgparts-com\public\stock\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2126638D-1AC3-4474-8E97-770B680CC4BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF46619D-38F8-4B26-B53F-1965C1FAB56F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{F3F29AF0-AF8F-4A3D-8182-67B847FBB111}"/>
   </bookViews>
@@ -47,9 +47,6 @@
     <t>oe</t>
   </si>
   <si>
-    <t xml:space="preserve"> brand</t>
-  </si>
-  <si>
     <t>model</t>
   </si>
   <si>
@@ -81,6 +78,10 @@
   </si>
   <si>
     <t>demo row</t>
+  </si>
+  <si>
+    <t>brand</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -467,7 +468,7 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -488,45 +489,45 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>10</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>11</v>
-      </c>
-      <c r="E2" t="s">
-        <v>12</v>
       </c>
       <c r="F2">
         <v>2018</v>
       </c>
       <c r="G2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" t="s">
         <v>13</v>
-      </c>
-      <c r="H2" t="s">
-        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>